<commit_message>
FARM Gamma LTI done
</commit_message>
<xml_diff>
--- a/tests/integration_tests/ARMA/Sine_24h/Data_24h_function.xlsx
+++ b/tests/integration_tests/ARMA/Sine_24h/Data_24h_function.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\wanghy_fork\HERON\tests\integration_tests\ARMA\Sine_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\wanghy_fork\HERON\tests\integration_tests\ARMA\Sine_24h\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B56A55-2231-4AE6-9D82-E928832E0A70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDC393E-D1CE-4A1B-9F08-0E6FC7666F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43920" yWindow="9975" windowWidth="9165" windowHeight="15435" activeTab="2" xr2:uid="{D61530F6-2741-4636-AC6C-BF1700677F29}"/>
+    <workbookView xWindow="43830" yWindow="870" windowWidth="16200" windowHeight="28035" activeTab="2" xr2:uid="{D61530F6-2741-4636-AC6C-BF1700677F29}"/>
   </bookViews>
   <sheets>
     <sheet name="How many to Charge" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1755,7 +1756,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C27"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,7 +1771,7 @@
         <v>6</v>
       </c>
       <c r="C1">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1778,7 +1779,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>-1130</v>
+        <v>-1147.5</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1813,23 +1814,23 @@
       </c>
       <c r="C4" s="3">
         <f>C$1*SIN(PI()/12*B4)+C$2</f>
-        <v>-1130</v>
+        <v>-1147.5</v>
       </c>
       <c r="D4" s="2">
         <f>(-1180.838-C4)</f>
-        <v>-50.837999999999965</v>
+        <v>-33.337999999999965</v>
       </c>
       <c r="E4" s="2">
         <f>SUM(D$4:D4)</f>
-        <v>-50.837999999999965</v>
+        <v>-33.337999999999965</v>
       </c>
       <c r="F4" s="2">
         <f>C$1*SIN(PI()/12*B4)+C$2</f>
-        <v>-1130</v>
+        <v>-1147.5</v>
       </c>
       <c r="G4" s="2">
         <f>C$1*SIN(PI()/12*B4)+C$2</f>
-        <v>-1130</v>
+        <v>-1147.5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1841,23 +1842,23 @@
       </c>
       <c r="C5" s="3">
         <f t="shared" ref="C5:C27" si="0">C$1*SIN(PI()/12*B5)+C$2</f>
-        <v>-1109.2944763917983</v>
+        <v>-1128.0885716173109</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ref="D5:D27" si="1">(-1180.838-C5)</f>
-        <v>-71.543523608201667</v>
+        <v>-52.749428382689075</v>
       </c>
       <c r="E5" s="2">
         <f>SUM(D$4:D5)</f>
-        <v>-122.38152360820163</v>
+        <v>-86.087428382689041</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" ref="F5:F27" si="2">C$1*SIN(PI()/12*B5)+C$2</f>
-        <v>-1109.2944763917983</v>
+        <v>-1128.0885716173109</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" ref="G5:G27" si="3">C$1*SIN(PI()/12*B5)+C$2</f>
-        <v>-1109.2944763917983</v>
+        <v>-1128.0885716173109</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1869,23 +1870,23 @@
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>-1090</v>
+        <v>-1110</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="1"/>
-        <v>-90.837999999999965</v>
+        <v>-70.837999999999965</v>
       </c>
       <c r="E6" s="2">
         <f>SUM(D$4:D6)</f>
-        <v>-213.2195236082016</v>
+        <v>-156.92542838268901</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="2"/>
-        <v>-1090</v>
+        <v>-1110</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="3"/>
-        <v>-1090</v>
+        <v>-1110</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1897,23 +1898,23 @@
       </c>
       <c r="C7" s="3">
         <f t="shared" si="0"/>
-        <v>-1073.4314575050762</v>
+        <v>-1094.4669914110088</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="1"/>
-        <v>-107.40654249492377</v>
+        <v>-86.371008588991117</v>
       </c>
       <c r="E7" s="2">
         <f>SUM(D$4:D7)</f>
-        <v>-320.62606610312537</v>
+        <v>-243.29643697168012</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="2"/>
-        <v>-1073.4314575050762</v>
+        <v>-1094.4669914110088</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="3"/>
-        <v>-1073.4314575050762</v>
+        <v>-1094.4669914110088</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1925,23 +1926,23 @@
       </c>
       <c r="C8" s="3">
         <f t="shared" si="0"/>
-        <v>-1060.7179676972448</v>
+        <v>-1082.548094716167</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="1"/>
-        <v>-120.12003230275513</v>
+        <v>-98.289905283832923</v>
       </c>
       <c r="E8" s="2">
         <f>SUM(D$4:D8)</f>
-        <v>-440.7460984058805</v>
+        <v>-341.58634225551305</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="2"/>
-        <v>-1060.7179676972448</v>
+        <v>-1082.548094716167</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="3"/>
-        <v>-1060.7179676972448</v>
+        <v>-1082.548094716167</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1953,23 +1954,23 @@
       </c>
       <c r="C9" s="3">
         <f t="shared" si="0"/>
-        <v>-1052.7259338968745</v>
+        <v>-1075.05556302832</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>-128.11206610312547</v>
+        <v>-105.78243697168</v>
       </c>
       <c r="E9" s="2">
         <f>SUM(D$4:D9)</f>
-        <v>-568.85816450900597</v>
+        <v>-447.36877922719304</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="2"/>
-        <v>-1052.7259338968745</v>
+        <v>-1075.05556302832</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="3"/>
-        <v>-1052.7259338968745</v>
+        <v>-1075.05556302832</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1981,23 +1982,23 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" si="0"/>
-        <v>-1050</v>
+        <v>-1072.5</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>-130.83799999999997</v>
+        <v>-108.33799999999997</v>
       </c>
       <c r="E10" s="2">
         <f>SUM(D$4:D10)</f>
-        <v>-699.69616450900594</v>
+        <v>-555.70677922719301</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="2"/>
-        <v>-1050</v>
+        <v>-1072.5</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="3"/>
-        <v>-1050</v>
+        <v>-1072.5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2009,23 +2010,23 @@
       </c>
       <c r="C11" s="3">
         <f t="shared" si="0"/>
-        <v>-1052.7259338968745</v>
+        <v>-1075.05556302832</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>-128.11206610312547</v>
+        <v>-105.78243697168</v>
       </c>
       <c r="E11" s="2">
         <f>SUM(D$4:D11)</f>
-        <v>-827.80823061213141</v>
+        <v>-661.48921619887301</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="2"/>
-        <v>-1052.7259338968745</v>
+        <v>-1075.05556302832</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="3"/>
-        <v>-1052.7259338968745</v>
+        <v>-1075.05556302832</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2037,23 +2038,23 @@
       </c>
       <c r="C12" s="3">
         <f t="shared" si="0"/>
-        <v>-1060.7179676972448</v>
+        <v>-1082.548094716167</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>-120.12003230275513</v>
+        <v>-98.289905283832923</v>
       </c>
       <c r="E12" s="2">
         <f>SUM(D$4:D12)</f>
-        <v>-947.92826291488655</v>
+        <v>-759.77912148270593</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="2"/>
-        <v>-1060.7179676972448</v>
+        <v>-1082.548094716167</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="3"/>
-        <v>-1060.7179676972448</v>
+        <v>-1082.548094716167</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2065,23 +2066,23 @@
       </c>
       <c r="C13" s="3">
         <f t="shared" si="0"/>
-        <v>-1073.4314575050762</v>
+        <v>-1094.4669914110088</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>-107.40654249492377</v>
+        <v>-86.371008588991117</v>
       </c>
       <c r="E13" s="2">
         <f>SUM(D$4:D13)</f>
-        <v>-1055.3348054098103</v>
+        <v>-846.15013007169705</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="2"/>
-        <v>-1073.4314575050762</v>
+        <v>-1094.4669914110088</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="3"/>
-        <v>-1073.4314575050762</v>
+        <v>-1094.4669914110088</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2093,23 +2094,23 @@
       </c>
       <c r="C14" s="3">
         <f t="shared" si="0"/>
-        <v>-1090</v>
+        <v>-1110</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
-        <v>-90.837999999999965</v>
+        <v>-70.837999999999965</v>
       </c>
       <c r="E14" s="2">
         <f>SUM(D$4:D14)</f>
-        <v>-1146.1728054098103</v>
+        <v>-916.98813007169701</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="2"/>
-        <v>-1090</v>
+        <v>-1110</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="3"/>
-        <v>-1090</v>
+        <v>-1110</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2121,23 +2122,23 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" si="0"/>
-        <v>-1109.2944763917983</v>
+        <v>-1128.0885716173109</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="1"/>
-        <v>-71.543523608201667</v>
+        <v>-52.749428382689075</v>
       </c>
       <c r="E15" s="2">
         <f>SUM(D$4:D15)</f>
-        <v>-1217.7163290180119</v>
+        <v>-969.73755845438609</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="2"/>
-        <v>-1109.2944763917983</v>
+        <v>-1128.0885716173109</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="3"/>
-        <v>-1109.2944763917983</v>
+        <v>-1128.0885716173109</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2149,23 +2150,23 @@
       </c>
       <c r="C16" s="3">
         <f t="shared" si="0"/>
-        <v>-1130</v>
+        <v>-1147.5</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>-50.837999999999965</v>
+        <v>-33.337999999999965</v>
       </c>
       <c r="E16" s="2">
         <f>SUM(D$4:D16)</f>
-        <v>-1268.5543290180119</v>
+        <v>-1003.0755584543861</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="2"/>
-        <v>-1130</v>
+        <v>-1147.5</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="3"/>
-        <v>-1130</v>
+        <v>-1147.5</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2177,23 +2178,23 @@
       </c>
       <c r="C17" s="3">
         <f t="shared" si="0"/>
-        <v>-1150.7055236082017</v>
+        <v>-1166.9114283826891</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>-30.132476391798264</v>
+        <v>-13.926571617310856</v>
       </c>
       <c r="E17" s="2">
         <f>SUM(D$4:D17)</f>
-        <v>-1298.6868054098102</v>
+        <v>-1017.0021300716969</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="2"/>
-        <v>-1150.7055236082017</v>
+        <v>-1166.9114283826891</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="3"/>
-        <v>-1150.7055236082017</v>
+        <v>-1166.9114283826891</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2205,23 +2206,23 @@
       </c>
       <c r="C18" s="3">
         <f t="shared" si="0"/>
-        <v>-1170</v>
+        <v>-1185</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>-10.837999999999965</v>
+        <v>4.1620000000000346</v>
       </c>
       <c r="E18" s="2">
         <f>SUM(D$4:D18)</f>
-        <v>-1309.5248054098101</v>
+        <v>-1012.8401300716969</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="2"/>
-        <v>-1170</v>
+        <v>-1185</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="3"/>
-        <v>-1170</v>
+        <v>-1185</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2233,23 +2234,23 @@
       </c>
       <c r="C19" s="3">
         <f t="shared" si="0"/>
-        <v>-1186.5685424949238</v>
+        <v>-1200.5330085889909</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
-        <v>5.7305424949238386</v>
+        <v>19.695008588990959</v>
       </c>
       <c r="E19" s="2">
         <f>SUM(D$4:D19)</f>
-        <v>-1303.7942629148863</v>
+        <v>-993.14512148270592</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="2"/>
-        <v>-1186.5685424949238</v>
+        <v>-1200.5330085889909</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="3"/>
-        <v>-1186.5685424949238</v>
+        <v>-1200.5330085889909</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2261,23 +2262,23 @@
       </c>
       <c r="C20" s="3">
         <f t="shared" si="0"/>
-        <v>-1199.2820323027552</v>
+        <v>-1212.451905283833</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="1"/>
-        <v>18.444032302755204</v>
+        <v>31.613905283832992</v>
       </c>
       <c r="E20" s="2">
         <f>SUM(D$4:D20)</f>
-        <v>-1285.3502306121311</v>
+        <v>-961.53121619887293</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="2"/>
-        <v>-1199.2820323027552</v>
+        <v>-1212.451905283833</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="3"/>
-        <v>-1199.2820323027552</v>
+        <v>-1212.451905283833</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2289,23 +2290,23 @@
       </c>
       <c r="C21" s="3">
         <f t="shared" si="0"/>
-        <v>-1207.2740661031255</v>
+        <v>-1219.94443697168</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="1"/>
-        <v>26.43606610312554</v>
+        <v>39.106436971680068</v>
       </c>
       <c r="E21" s="2">
         <f>SUM(D$4:D21)</f>
-        <v>-1258.9141645090056</v>
+        <v>-922.42477922719286</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>-1207.2740661031255</v>
+        <v>-1219.94443697168</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="3"/>
-        <v>-1207.2740661031255</v>
+        <v>-1219.94443697168</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2317,23 +2318,23 @@
       </c>
       <c r="C22" s="3">
         <f t="shared" si="0"/>
-        <v>-1210</v>
+        <v>-1222.5</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="1"/>
-        <v>29.162000000000035</v>
+        <v>41.662000000000035</v>
       </c>
       <c r="E22" s="2">
         <f>SUM(D$4:D22)</f>
-        <v>-1229.7521645090055</v>
+        <v>-880.76277922719282</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="2"/>
-        <v>-1210</v>
+        <v>-1222.5</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="3"/>
-        <v>-1210</v>
+        <v>-1222.5</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2345,23 +2346,23 @@
       </c>
       <c r="C23" s="3">
         <f t="shared" si="0"/>
-        <v>-1207.2740661031255</v>
+        <v>-1219.94443697168</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="1"/>
-        <v>26.43606610312554</v>
+        <v>39.106436971680068</v>
       </c>
       <c r="E23" s="2">
         <f>SUM(D$4:D23)</f>
-        <v>-1203.31609840588</v>
+        <v>-841.65634225551275</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="2"/>
-        <v>-1207.2740661031255</v>
+        <v>-1219.94443697168</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="3"/>
-        <v>-1207.2740661031255</v>
+        <v>-1219.94443697168</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2373,23 +2374,23 @@
       </c>
       <c r="C24" s="3">
         <f t="shared" si="0"/>
-        <v>-1199.2820323027552</v>
+        <v>-1212.451905283833</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="1"/>
-        <v>18.444032302755204</v>
+        <v>31.613905283832992</v>
       </c>
       <c r="E24" s="2">
         <f>SUM(D$4:D24)</f>
-        <v>-1184.8720661031248</v>
+        <v>-810.04243697167976</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="2"/>
-        <v>-1199.2820323027552</v>
+        <v>-1212.451905283833</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="3"/>
-        <v>-1199.2820323027552</v>
+        <v>-1212.451905283833</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2401,23 +2402,23 @@
       </c>
       <c r="C25" s="3">
         <f t="shared" si="0"/>
-        <v>-1186.5685424949238</v>
+        <v>-1200.5330085889912</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="1"/>
-        <v>5.7305424949238386</v>
+        <v>19.695008588991186</v>
       </c>
       <c r="E25" s="2">
         <f>SUM(D$4:D25)</f>
-        <v>-1179.1415236082009</v>
+        <v>-790.34742838268858</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="2"/>
-        <v>-1186.5685424949238</v>
+        <v>-1200.5330085889912</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" si="3"/>
-        <v>-1186.5685424949238</v>
+        <v>-1200.5330085889912</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2429,23 +2430,23 @@
       </c>
       <c r="C26" s="3">
         <f t="shared" si="0"/>
-        <v>-1170</v>
+        <v>-1185</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="1"/>
-        <v>-10.837999999999965</v>
+        <v>4.1620000000000346</v>
       </c>
       <c r="E26" s="2">
         <f>SUM(D$4:D26)</f>
-        <v>-1189.9795236082009</v>
+        <v>-786.18542838268854</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="2"/>
-        <v>-1170</v>
+        <v>-1185</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" si="3"/>
-        <v>-1170</v>
+        <v>-1185</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2457,23 +2458,23 @@
       </c>
       <c r="C27" s="3">
         <f t="shared" si="0"/>
-        <v>-1150.7055236082017</v>
+        <v>-1166.9114283826891</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="1"/>
-        <v>-30.132476391798264</v>
+        <v>-13.926571617310856</v>
       </c>
       <c r="E27" s="2">
         <f>SUM(D$4:D27)</f>
-        <v>-1220.1119999999992</v>
+        <v>-800.1119999999994</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" si="2"/>
-        <v>-1150.7055236082017</v>
+        <v>-1166.9114283826891</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" si="3"/>
-        <v>-1150.7055236082017</v>
+        <v>-1166.9114283826891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>